<commit_message>
Add advent of code
</commit_message>
<xml_diff>
--- a/Leetcode/Thinking_process/Leetcode NoteBook/LeetCode_Whiteboard/Leetcode.xlsx
+++ b/Leetcode/Thinking_process/Leetcode NoteBook/LeetCode_Whiteboard/Leetcode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Nguyen\Coding\C++\Competitive_programming\Leetcode\Thinking_process\Leetcode NoteBook\LeetCode_Whiteboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B2B66EDE-CB44-42FC-AFF2-22208CE0016E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0F9EFAB-40A8-4041-9D67-1694BFE494E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3036" yWindow="3036" windowWidth="17280" windowHeight="8964" xr2:uid="{5619DD07-ACFA-46F6-80A6-6DEA1884F055}"/>
   </bookViews>
@@ -33,6 +33,44 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+  <si>
+    <t xml:space="preserve">Topics </t>
+  </si>
+  <si>
+    <t>Algorithm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Question </t>
+  </si>
+  <si>
+    <t>Array</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Backtracking, Bit manipulation </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Subset II </t>
+  </si>
+  <si>
+    <t>Solution</t>
+  </si>
+  <si>
+    <t>Level</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>Possible alternatives</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -382,12 +420,62 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DD99BE9-897A-4D31-930A-0DD62EF5A28E}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="3" max="3" width="29.109375" customWidth="1"/>
+    <col min="4" max="4" width="51.21875" customWidth="1"/>
+    <col min="6" max="6" width="44.44140625" customWidth="1"/>
+    <col min="7" max="7" width="32.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>90</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>